<commit_message>
just changed pom.xml and testcase3
</commit_message>
<xml_diff>
--- a/OpencartV121/testData/Opencart_LoginData.xlsx
+++ b/OpencartV121/testData/Opencart_LoginData.xlsx
@@ -1,87 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8E638BAF-3E4B-4B9F-9F6F-552582B64E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\myworkspaces\seleniumwebdriver\OpencartV121\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47704AFE-A492-43CB-82D7-6A46F57DC3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DB08A899-3D50-4627-AA9E-9D277DF4F032}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>lakshmi@yahoo.com</t>
+  </si>
+  <si>
+    <t>Lakshmi</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>laksh@yahoo.com</t>
+  </si>
+  <si>
+    <t>Laxmi</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>laks@yahoo.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>pavanoltraining@gmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
   <si>
     <t>abc123@gmail.com</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>res</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>laks@yahoo.com</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>Invalid</t>
-  </si>
-  <si>
-    <t>laksh@yahoo.com</t>
-  </si>
-  <si>
-    <t>Lakshmi</t>
-  </si>
-  <si>
-    <t>Laxmi</t>
-  </si>
-  <si>
-    <t>lakshmi@yahoo.com</t>
-  </si>
-  <si>
-    <t>480@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -89,7 +94,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -108,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,15 +136,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -154,39 +199,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -238,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -349,6 +394,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -357,13 +409,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -428,127 +473,118 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D0F166-CFB9-44B7-AAF7-428B5CD21237}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>1234123412</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{105ECA89-2C64-4296-AA1A-5E3DA31ED440}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{23F9B6B4-CC45-4F99-8B19-6F1FB5998677}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{498DA6CB-8522-40D3-9E9E-0C9AF85BBB20}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{BBE337FE-CD02-4751-BA7C-4305C3C09580}"/>
-    <hyperlink ref="A3" r:id="rId5" xr:uid="{6E2791E6-FBF8-4535-BFD8-DE28E244E260}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{39D93D16-C102-40D9-B1A5-F772FEC2FB1A}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{B4FF4FF2-C3C7-488B-A3F2-29DB9D3EA93F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>